<commit_message>
Add much to brain board schematic
</commit_message>
<xml_diff>
--- a/BOMs/sinking-clock-BOM-v2.xlsx
+++ b/BOMs/sinking-clock-BOM-v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C577C71-E569-4C2C-9428-82804957857E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507D5346-1D7F-44FF-8D30-FAE4AFBCCE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brain PCB Assembly" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="302">
   <si>
     <t>Quantity</t>
   </si>
@@ -929,6 +929,21 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/cui-devices/PJ-002BH-SMT-TR/404626</t>
+  </si>
+  <si>
+    <t>res</t>
+  </si>
+  <si>
+    <t>cap</t>
+  </si>
+  <si>
+    <t>ferrite bead</t>
+  </si>
+  <si>
+    <t>32.768 kHz crystal oscillator</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/ecs-inc/ECS-327-12-5-12R-TR/8593595</t>
   </si>
 </sst>
 </file>
@@ -1469,9 +1484,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535EBE7C-EB1B-4F48-8827-B2C8DF8DD54E}">
   <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1688,6 +1703,9 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>297</v>
+      </c>
       <c r="I15" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1695,112 +1713,123 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>298</v>
+      </c>
       <c r="I16" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>299</v>
+      </c>
       <c r="I17" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>300</v>
+      </c>
       <c r="I18" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="J18" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I19" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I20" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I21" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I22" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I23" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I24" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I25" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I26" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I27" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I28" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I29" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I30" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I31" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I32" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2251,9 +2280,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF30F9AC-3655-4B8A-AD78-25E473D1BEC8}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:J17"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5696,9 +5725,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B494BF-8FB3-4F10-BF9B-C1AB6CBBBD39}">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>